<commit_message>
Medium assessment changes updated
</commit_message>
<xml_diff>
--- a/final-framework-testng/resources/RegistrationTestData.xlsx
+++ b/final-framework-testng/resources/RegistrationTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{BAA25481-C40A-4863-BAEA-B947D954EBCB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{24202910-7468-44AA-B55D-EC60B22779E9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="1100" windowWidth="14420" windowHeight="10830" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1440" yWindow="1440" windowWidth="19440" windowHeight="11060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,10 +35,10 @@
     <t>nov22nov</t>
   </si>
   <si>
-    <t>Ashwini12</t>
-  </si>
-  <si>
-    <t>ashwini1234@gmail.com</t>
+    <t>sonu</t>
+  </si>
+  <si>
+    <t>sonu445@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -370,16 +370,10 @@
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="10.1796875" customWidth="1"/>
-    <col min="2" max="2" width="9.7265625" customWidth="1"/>
-    <col min="3" max="3" width="18.54296875" customWidth="1"/>
-    <col min="4" max="4" width="13.6328125" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
@@ -412,7 +406,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C1" r:id="rId1" xr:uid="{DFADA8E6-3660-4EA4-9AFB-79BBC4F94153}"/>
+    <hyperlink ref="C1" r:id="rId1" xr:uid="{0749C477-09F3-4BF5-8AAB-032C089BEB53}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>